<commit_message>
Config updated - m-subcat
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\My_love\Documents\GitHub\DND_MaterialHealth\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B843FFA-6C76-4758-A586-9B1B2A6C0DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A4D3A6-4931-4F34-ACE7-BE9BA5AAEDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -270,10 +270,10 @@
     <t>filename</t>
   </si>
   <si>
-    <t>Status,Mat_Hlth_Cat,Mat_Hlt_Sub-Cat,Mat_Hlth_Sub-Sub_Cat,Tranche_1?,Storage_Location_Group,Last_Demand_Year,Assigned_Year,Line_Value,Price,Blocked,Quality_Inspection,Lead_EPM,Mark_As_Hazmat,Storage_Medium,Size_factor,Storage_Bin,Count,Cubic_Metres,25_CFSD_Bin_Structure,Transit_Bin,Robot_Message,Sheet</t>
-  </si>
-  <si>
     <t>25 CFSD Mat Hlth</t>
+  </si>
+  <si>
+    <t>Status,Mat_Hlth_Cat,Mat_Hlt_Sub_Cat,Mat_Hlth_Sub_Sub_Cat,Tranche_1?,Storage_Location_Group,Last_Demand_Year,Assigned_Year,Line_Value,Price,Blocked,Quality_Inspection,Lead_EPM,Mark_As_Hazmat,Storage_Medium,Size_factor,Storage_Bin,Count,Cubic_Metres,25_CFSD_Bin_Structure,Transit_Bin,Robot_Message,Sheet</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -941,7 +941,7 @@
         <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1926,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2057,7 +2057,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>57</v>

</xml_diff>